<commit_message>
fix bug for incorrect chart
</commit_message>
<xml_diff>
--- a/files/Master_Table.xlsx
+++ b/files/Master_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkeeley/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkeeley/src/Spoofy/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41923600-4727-2544-B244-0E80C5B087EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC835B1-CF8B-1C49-BFDA-09F160961AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67020" yWindow="-5600" windowWidth="36200" windowHeight="28160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="76020" yWindow="-5820" windowWidth="27200" windowHeight="28160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,23 +261,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -285,192 +269,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -752,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:JR199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33094,14 +32892,14 @@
       <c r="JR114"/>
     </row>
     <row r="115" spans="1:278" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C115" s="2">
-        <v>8</v>
+      <c r="C115" s="4">
+        <v>7</v>
       </c>
       <c r="D115"/>
       <c r="E115"/>
@@ -57408,7 +57206,7 @@
     <sortCondition ref="A2:A199"/>
   </sortState>
   <conditionalFormatting sqref="B42:B44">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
python3 spoofy.py -d cwrt.xyz
</commit_message>
<xml_diff>
--- a/files/Master_Table.xlsx
+++ b/files/Master_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkeeley/src/Spoofy/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC835B1-CF8B-1C49-BFDA-09F160961AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB8842E-8B0D-8C47-8939-83D5C427C2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="76020" yWindow="-5820" windowWidth="27200" windowHeight="28160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:JR199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32899,7 +32899,7 @@
         <v>2</v>
       </c>
       <c r="C115" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D115"/>
       <c r="E115"/>

</xml_diff>